<commit_message>
docs: rename mention_name to key and target_age to target_audience
Update prop naming across CLAUDE.md and api/text-generation specs:
- mention_name → key (serves as identifier like id)
- target_age → target_audience (consistent with DB schema)
- Add missing fields to agents table: key, knowledge, lens
- Add type field to locations table
</commit_message>
<xml_diff>
--- a/CoreDB.xlsx
+++ b/CoreDB.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="274">
   <si>
     <t xml:space="preserve">FIelds</t>
   </si>
@@ -567,7 +567,7 @@
     <t xml:space="preserve">characters[]</t>
   </si>
   <si>
-    <t xml:space="preserve">mention_name</t>
+    <t xml:space="preserve">key</t>
   </si>
   <si>
     <t xml:space="preserve">để gọi ra đồng nhất</t>
@@ -769,9 +769,6 @@
     <t xml:space="preserve">Cat/Dog/Pig/Old man/Car/....</t>
   </si>
   <si>
-    <t xml:space="preserve">TINYINT</t>
-  </si>
-  <si>
     <t xml:space="preserve">(human, animal, plant, item)</t>
   </si>
   <si>
@@ -784,7 +781,9 @@
     <t xml:space="preserve">locations</t>
   </si>
   <si>
-    <t xml:space="preserve">những địa danh cụ thể: thành phố, địa danh,...</t>
+    <t xml:space="preserve">những địa danh cụ thể: thành phố, địa danh,... 
+dùng để tác động lên yếu tố nội dung văn hoá và mô tả hình ảnh hơn là tạo hình
+tạo hình cụ thể nằm ở stages</t>
   </si>
   <si>
     <t xml:space="preserve">nation</t>
@@ -793,7 +792,14 @@
     <t xml:space="preserve">city</t>
   </si>
   <si>
+    <t xml:space="preserve">0: ở trái đất, địa điểm có thật. 1: địa điểm hư cấu hoặc ngoài trái đất</t>
+  </si>
+  <si>
     <t xml:space="preserve">eras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dùng để tác động lên yếu tố nội dung văn hoá và mô tả hình ảnh hơn là tạo hình
+tạo hình cụ thể nằm ở stages</t>
   </si>
   <si>
     <t xml:space="preserve">environments</t>
@@ -817,13 +823,22 @@
     <t xml:space="preserve">agents</t>
   </si>
   <si>
+    <t xml:space="preserve">Để orchestrator đọc và gọi khi cần</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knowledge</t>
+  </si>
+  <si>
     <t xml:space="preserve">instruction</t>
   </si>
   <si>
-    <t xml:space="preserve">Để orchestrator đọc và gọi khi cần</t>
+    <t xml:space="preserve">lens</t>
   </si>
   <si>
-    <t xml:space="preserve">1: story agents, 2: characters, 3: parents, 4: children</t>
+    <t xml:space="preserve">xu hướng riêng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: storyteller, 2: artdirector, 3: wordsmith, 4: reviewer, 5: parents, 6: children, 7: characters</t>
   </si>
   <si>
     <t xml:space="preserve">ai_requests</t>
@@ -1223,8 +1238,8 @@
   </sheetPr>
   <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E93" activeCellId="0" sqref="E93"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F60" activeCellId="0" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4855,7 +4870,7 @@
   <dimension ref="A1:AD1063"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
@@ -5237,7 +5252,7 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
@@ -5247,7 +5262,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="6" t="s">
         <v>104</v>
       </c>
       <c r="I11" s="3"/>
@@ -38677,7 +38692,7 @@
   </sheetPr>
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -38979,7 +38994,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -39041,10 +39056,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39055,12 +39070,12 @@
         <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39108,10 +39123,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39140,7 +39155,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>8</v>
@@ -39148,157 +39163,163 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>5</v>
+      <c r="F25" s="3" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="3" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="16" t="s">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D31" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
-        <v>253</v>
-      </c>
-    </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>5</v>
+      <c r="A33" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="3" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="16" t="s">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C40" s="3"/>
-    </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A41" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>13</v>
@@ -39306,162 +39327,170 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>8</v>
+        <v>29</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="3" t="s">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D48" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F47" s="6"/>
-    </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E48" s="6" t="s">
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="3"/>
-      <c r="F49" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="3"/>
       <c r="F50" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="3"/>
       <c r="F51" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E53" s="3" t="s">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F53" s="6"/>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E54" s="5" t="s">
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E55" s="5"/>
-      <c r="F55" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="F55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3"/>
       <c r="E56" s="5"/>
       <c r="F56" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G56" s="6"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3"/>
-      <c r="E57" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="E58" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
-      <c r="E59" s="3"/>
+      <c r="E59" s="5"/>
       <c r="F59" s="3" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="6"/>
+      <c r="A60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G60" s="3"/>
+    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="6"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E61" s="5"/>
-      <c r="F61" s="3" t="s">
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="5"/>
+      <c r="F62" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D62" s="6" t="s">
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F62" s="6"/>
-    </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D63" s="6"/>
-      <c r="E63" s="6" t="s">
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D64" s="6"/>
+      <c r="E64" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F63" s="5"/>
-    </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E64" s="3"/>
-      <c r="F64" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="3"/>
       <c r="F65" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="3"/>
       <c r="F66" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="3"/>
       <c r="F67" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="3"/>
+      <c r="F68" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E68" s="3" t="s">
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F68" s="6"/>
+      <c r="F69" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -39480,7 +39509,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -39499,7 +39528,7 @@
         <v>93</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -39527,7 +39556,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39556,7 +39585,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
@@ -39564,7 +39593,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39585,101 +39614,139 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>260</v>
+        <v>177</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>258</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>9</v>
+        <v>262</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>261</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="F17" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>8</v>
+      <c r="A22" s="3" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="3" t="s">
-        <v>264</v>
+        <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>265</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
-        <v>266</v>
+        <v>76</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="3" t="s">
-        <v>267</v>
+        <v>102</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="3" t="s">
         <v>268</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -39702,7 +39769,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -39718,7 +39785,7 @@
         <v>93</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -39748,7 +39815,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39801,7 +39868,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
update snapshot manuscript field
</commit_message>
<xml_diff>
--- a/CoreDB.xlsx
+++ b/CoreDB.xlsx
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="314">
   <si>
     <t xml:space="preserve">FIelds</t>
   </si>
@@ -406,7 +406,7 @@
     <t xml:space="preserve">manual save hay autobackup save</t>
   </si>
   <si>
-    <t xml:space="preserve">manuscripts[]</t>
+    <t xml:space="preserve">manuscript</t>
   </si>
   <si>
     <t xml:space="preserve">docs[]</t>
@@ -473,9 +473,6 @@
   </si>
   <si>
     <t xml:space="preserve">1: dps, 0: non-dps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manuscript</t>
   </si>
   <si>
     <t xml:space="preserve">bê từ docs manuscript sang</t>
@@ -5067,9 +5064,9 @@
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J34" activeCellId="0" sqref="J34"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5407,7 +5404,7 @@
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -6662,7 +6659,7 @@
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -6673,7 +6670,7 @@
         <v>116</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -6813,7 +6810,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
@@ -6953,7 +6950,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
@@ -7018,7 +7015,7 @@
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -7054,7 +7051,7 @@
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -7129,7 +7126,7 @@
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
@@ -7293,7 +7290,7 @@
         <v>53</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
@@ -7335,7 +7332,7 @@
         <v>53</v>
       </c>
       <c r="J65" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
@@ -7377,7 +7374,7 @@
         <v>53</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
@@ -7419,7 +7416,7 @@
         <v>53</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
@@ -7451,7 +7448,7 @@
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
@@ -7459,7 +7456,7 @@
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
       <c r="J68" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
@@ -7498,10 +7495,10 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
       <c r="I69" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J69" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
@@ -7540,10 +7537,10 @@
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
       <c r="I70" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
@@ -7575,7 +7572,7 @@
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
@@ -7689,7 +7686,7 @@
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
@@ -7727,7 +7724,7 @@
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -7804,7 +7801,7 @@
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
@@ -7842,16 +7839,16 @@
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
       <c r="H78" s="6"/>
       <c r="I78" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J78" s="10" t="s">
         <v>135</v>
-      </c>
-      <c r="J78" s="10" t="s">
-        <v>136</v>
       </c>
       <c r="K78" s="6"/>
       <c r="L78" s="6"/>
@@ -7883,7 +7880,7 @@
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E79" s="6"/>
       <c r="F79" s="6"/>
@@ -7960,13 +7957,13 @@
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
       <c r="I81" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J81" s="10"/>
       <c r="K81" s="6"/>
@@ -8000,16 +7997,16 @@
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
       <c r="H82" s="6"/>
       <c r="I82" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J82" s="10" t="s">
         <v>135</v>
-      </c>
-      <c r="J82" s="10" t="s">
-        <v>136</v>
       </c>
       <c r="K82" s="6"/>
       <c r="L82" s="6"/>
@@ -8238,7 +8235,7 @@
       <c r="G88" s="6"/>
       <c r="H88" s="6"/>
       <c r="I88" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -8319,7 +8316,7 @@
         <v>53</v>
       </c>
       <c r="J90" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K90" s="6"/>
       <c r="L90" s="6"/>
@@ -8361,7 +8358,7 @@
         <v>53</v>
       </c>
       <c r="J91" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K91" s="6"/>
       <c r="L91" s="6"/>
@@ -8403,7 +8400,7 @@
         <v>53</v>
       </c>
       <c r="J92" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K92" s="6"/>
       <c r="L92" s="6"/>
@@ -8445,7 +8442,7 @@
         <v>53</v>
       </c>
       <c r="J93" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K93" s="6"/>
       <c r="L93" s="6"/>
@@ -8479,7 +8476,7 @@
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
       <c r="F94" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G94" s="10"/>
       <c r="H94" s="10"/>
@@ -8565,7 +8562,7 @@
         <v>53</v>
       </c>
       <c r="J96" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K96" s="6"/>
       <c r="L96" s="6"/>
@@ -8607,7 +8604,7 @@
         <v>53</v>
       </c>
       <c r="J97" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K97" s="6"/>
       <c r="L97" s="6"/>
@@ -8647,7 +8644,7 @@
       <c r="H98" s="6"/>
       <c r="I98" s="6"/>
       <c r="J98" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K98" s="6"/>
       <c r="L98" s="6"/>
@@ -8727,7 +8724,7 @@
       <c r="H100" s="6"/>
       <c r="I100" s="6"/>
       <c r="J100" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K100" s="6"/>
       <c r="L100" s="6"/>
@@ -8769,7 +8766,7 @@
         <v>53</v>
       </c>
       <c r="J101" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K101" s="6"/>
       <c r="L101" s="6"/>
@@ -8811,7 +8808,7 @@
         <v>53</v>
       </c>
       <c r="J102" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K102" s="6"/>
       <c r="L102" s="6"/>
@@ -8851,7 +8848,7 @@
       <c r="H103" s="6"/>
       <c r="I103" s="6"/>
       <c r="J103" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K103" s="6"/>
       <c r="L103" s="6"/>
@@ -8891,7 +8888,7 @@
       <c r="H104" s="6"/>
       <c r="I104" s="6"/>
       <c r="J104" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K104" s="6"/>
       <c r="L104" s="6"/>
@@ -8931,7 +8928,7 @@
       <c r="H105" s="6"/>
       <c r="I105" s="6"/>
       <c r="J105" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K105" s="6"/>
       <c r="L105" s="6"/>
@@ -8964,7 +8961,7 @@
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
       <c r="E106" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
@@ -9041,7 +9038,7 @@
       <c r="D108" s="6"/>
       <c r="E108" s="6"/>
       <c r="F108" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G108" s="6"/>
       <c r="H108" s="6"/>
@@ -9078,7 +9075,7 @@
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
       <c r="E109" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F109" s="6"/>
       <c r="G109" s="6"/>
@@ -9122,7 +9119,7 @@
       <c r="G110" s="6"/>
       <c r="H110" s="6"/>
       <c r="I110" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J110" s="6"/>
       <c r="K110" s="6"/>
@@ -9157,7 +9154,7 @@
       <c r="D111" s="6"/>
       <c r="E111" s="6"/>
       <c r="F111" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G111" s="6"/>
       <c r="H111" s="6"/>
@@ -9197,7 +9194,7 @@
       <c r="D112" s="6"/>
       <c r="E112" s="6"/>
       <c r="F112" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G112" s="6"/>
       <c r="H112" s="6"/>
@@ -9242,10 +9239,10 @@
       <c r="G113" s="6"/>
       <c r="H113" s="6"/>
       <c r="I113" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J113" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="J113" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="K113" s="6"/>
       <c r="L113" s="6"/>
@@ -9278,7 +9275,7 @@
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
       <c r="E114" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F114" s="6"/>
       <c r="G114" s="6"/>
@@ -9317,7 +9314,7 @@
       <c r="D115" s="6"/>
       <c r="E115" s="6"/>
       <c r="F115" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G115" s="6"/>
       <c r="H115" s="6"/>
@@ -9393,7 +9390,7 @@
       <c r="D117" s="6"/>
       <c r="E117" s="6"/>
       <c r="F117" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G117" s="6"/>
       <c r="H117" s="6"/>
@@ -9431,7 +9428,7 @@
       <c r="D118" s="6"/>
       <c r="E118" s="6"/>
       <c r="F118" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G118" s="10"/>
       <c r="H118" s="10"/>
@@ -9469,7 +9466,7 @@
       <c r="D119" s="6"/>
       <c r="E119" s="6"/>
       <c r="F119" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G119" s="10"/>
       <c r="H119" s="10"/>
@@ -9542,7 +9539,7 @@
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D121" s="6"/>
       <c r="E121" s="6"/>
@@ -9627,7 +9624,7 @@
       <c r="H123" s="6"/>
       <c r="I123" s="6"/>
       <c r="J123" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K123" s="6"/>
       <c r="L123" s="6"/>
@@ -9659,7 +9656,7 @@
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
       <c r="D124" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E124" s="6"/>
       <c r="F124" s="6"/>
@@ -9667,7 +9664,7 @@
       <c r="H124" s="6"/>
       <c r="I124" s="6"/>
       <c r="J124" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K124" s="6"/>
       <c r="L124" s="6"/>
@@ -9707,7 +9704,7 @@
       <c r="H125" s="6"/>
       <c r="I125" s="6"/>
       <c r="J125" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K125" s="6"/>
       <c r="L125" s="6"/>
@@ -9739,7 +9736,7 @@
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
       <c r="D126" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E126" s="6"/>
       <c r="F126" s="6"/>
@@ -9747,7 +9744,7 @@
       <c r="H126" s="6"/>
       <c r="I126" s="6"/>
       <c r="J126" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K126" s="6"/>
       <c r="L126" s="6"/>
@@ -9779,7 +9776,7 @@
       <c r="B127" s="6"/>
       <c r="C127" s="6"/>
       <c r="D127" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E127" s="6"/>
       <c r="F127" s="6"/>
@@ -9825,7 +9822,7 @@
       <c r="H128" s="6"/>
       <c r="I128" s="6"/>
       <c r="J128" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K128" s="6"/>
       <c r="L128" s="6"/>
@@ -9864,7 +9861,7 @@
         <v>53</v>
       </c>
       <c r="J129" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K129" s="6"/>
       <c r="L129" s="6"/>
@@ -9903,7 +9900,7 @@
         <v>53</v>
       </c>
       <c r="J130" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K130" s="6"/>
       <c r="L130" s="6"/>
@@ -9942,7 +9939,7 @@
         <v>53</v>
       </c>
       <c r="J131" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K131" s="6"/>
       <c r="L131" s="6"/>
@@ -9981,7 +9978,7 @@
         <v>53</v>
       </c>
       <c r="J132" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K132" s="6"/>
       <c r="L132" s="6"/>
@@ -10013,7 +10010,7 @@
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
       <c r="D133" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E133" s="6"/>
       <c r="I133" s="6" t="s">
@@ -10050,7 +10047,7 @@
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
       <c r="D134" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E134" s="6"/>
       <c r="F134" s="6"/>
@@ -10088,7 +10085,7 @@
       <c r="B135" s="6"/>
       <c r="C135" s="6"/>
       <c r="D135" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E135" s="6"/>
       <c r="F135" s="6"/>
@@ -10161,7 +10158,7 @@
       <c r="A137" s="6"/>
       <c r="B137" s="6"/>
       <c r="C137" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="6"/>
@@ -10200,7 +10197,7 @@
       <c r="B138" s="6"/>
       <c r="C138" s="6"/>
       <c r="D138" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E138" s="6"/>
       <c r="F138" s="6"/>
@@ -10238,7 +10235,7 @@
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
       <c r="D139" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E139" s="6"/>
       <c r="F139" s="6"/>
@@ -10276,7 +10273,7 @@
       <c r="B140" s="6"/>
       <c r="C140" s="6"/>
       <c r="D140" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E140" s="6"/>
       <c r="F140" s="6"/>
@@ -10284,7 +10281,7 @@
       <c r="H140" s="6"/>
       <c r="I140" s="6"/>
       <c r="J140" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K140" s="6"/>
       <c r="L140" s="6"/>
@@ -10316,7 +10313,7 @@
       <c r="B141" s="6"/>
       <c r="C141" s="6"/>
       <c r="D141" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E141" s="18"/>
       <c r="F141" s="14"/>
@@ -10362,7 +10359,7 @@
       <c r="H142" s="14"/>
       <c r="I142" s="6"/>
       <c r="J142" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K142" s="6"/>
       <c r="L142" s="6"/>
@@ -10591,7 +10588,7 @@
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
       <c r="D148" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E148" s="6"/>
       <c r="F148" s="6"/>
@@ -10599,7 +10596,7 @@
       <c r="H148" s="6"/>
       <c r="I148" s="6"/>
       <c r="J148" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K148" s="6"/>
       <c r="L148" s="6"/>
@@ -10631,14 +10628,14 @@
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
       <c r="D149" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E149" s="6"/>
       <c r="I149" s="6" t="s">
         <v>53</v>
       </c>
       <c r="J149" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K149" s="6"/>
       <c r="L149" s="6"/>
@@ -10670,14 +10667,14 @@
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
       <c r="D150" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E150" s="6"/>
       <c r="I150" s="6" t="s">
         <v>53</v>
       </c>
       <c r="J150" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K150" s="6"/>
       <c r="L150" s="6"/>
@@ -10709,14 +10706,14 @@
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
       <c r="D151" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E151" s="6"/>
       <c r="I151" s="6" t="s">
         <v>53</v>
       </c>
       <c r="J151" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K151" s="6"/>
       <c r="L151" s="6"/>
@@ -10781,7 +10778,7 @@
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B153" s="6" t="s">
         <v>20</v>
@@ -10823,7 +10820,7 @@
       <c r="A154" s="6"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="6"/>
@@ -10861,7 +10858,7 @@
       <c r="A155" s="6"/>
       <c r="B155" s="6"/>
       <c r="C155" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D155" s="6"/>
       <c r="E155" s="6"/>
@@ -10870,7 +10867,7 @@
       <c r="H155" s="6"/>
       <c r="I155" s="6"/>
       <c r="J155" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K155" s="6"/>
       <c r="L155" s="6"/>
@@ -10939,7 +10936,7 @@
       <c r="A157" s="6"/>
       <c r="B157" s="6"/>
       <c r="C157" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D157" s="6"/>
       <c r="E157" s="6"/>
@@ -11016,7 +11013,7 @@
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
       <c r="D159" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E159" s="6"/>
       <c r="F159" s="6"/>
@@ -11056,7 +11053,7 @@
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
       <c r="D160" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E160" s="6"/>
       <c r="F160" s="6"/>
@@ -11094,7 +11091,7 @@
       <c r="B161" s="6"/>
       <c r="C161" s="6"/>
       <c r="D161" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E161" s="6"/>
       <c r="F161" s="6"/>
@@ -11104,7 +11101,7 @@
         <v>57</v>
       </c>
       <c r="J161" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K161" s="6"/>
       <c r="L161" s="6"/>
@@ -11136,7 +11133,7 @@
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
       <c r="D162" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E162" s="6"/>
       <c r="F162" s="6"/>
@@ -11173,7 +11170,7 @@
       <c r="A163" s="6"/>
       <c r="B163" s="6"/>
       <c r="C163" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D163" s="6"/>
       <c r="E163" s="6"/>
@@ -11212,14 +11209,14 @@
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>
       <c r="D164" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E164" s="6"/>
       <c r="F164" s="6"/>
       <c r="G164" s="6"/>
       <c r="H164" s="6"/>
       <c r="I164" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J164" s="6"/>
       <c r="K164" s="6"/>
@@ -11252,14 +11249,14 @@
       <c r="B165" s="6"/>
       <c r="C165" s="6"/>
       <c r="D165" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E165" s="6"/>
       <c r="F165" s="6"/>
       <c r="G165" s="6"/>
       <c r="H165" s="6"/>
       <c r="I165" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J165" s="6"/>
       <c r="K165" s="6"/>
@@ -11292,14 +11289,14 @@
       <c r="B166" s="6"/>
       <c r="C166" s="6"/>
       <c r="D166" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E166" s="6"/>
       <c r="F166" s="6"/>
       <c r="G166" s="6"/>
       <c r="H166" s="6"/>
       <c r="I166" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J166" s="6"/>
       <c r="K166" s="6"/>
@@ -11332,14 +11329,14 @@
       <c r="B167" s="6"/>
       <c r="C167" s="6"/>
       <c r="D167" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E167" s="6"/>
       <c r="F167" s="6"/>
       <c r="G167" s="6"/>
       <c r="H167" s="6"/>
       <c r="I167" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J167" s="6"/>
       <c r="K167" s="6"/>
@@ -11372,14 +11369,14 @@
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
       <c r="D168" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E168" s="6"/>
       <c r="F168" s="6"/>
       <c r="G168" s="6"/>
       <c r="H168" s="6"/>
       <c r="I168" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J168" s="6"/>
       <c r="K168" s="6"/>
@@ -11412,14 +11409,14 @@
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
       <c r="D169" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E169" s="6"/>
       <c r="F169" s="6"/>
       <c r="G169" s="6"/>
       <c r="H169" s="6"/>
       <c r="I169" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J169" s="6"/>
       <c r="K169" s="6"/>
@@ -11452,14 +11449,14 @@
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
       <c r="D170" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E170" s="6"/>
       <c r="F170" s="6"/>
       <c r="G170" s="6"/>
       <c r="H170" s="6"/>
       <c r="I170" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J170" s="6"/>
       <c r="K170" s="6"/>
@@ -11492,14 +11489,14 @@
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
       <c r="D171" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E171" s="6"/>
       <c r="F171" s="6"/>
       <c r="G171" s="6"/>
       <c r="H171" s="6"/>
       <c r="I171" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J171" s="6"/>
       <c r="K171" s="6"/>
@@ -11531,7 +11528,7 @@
       <c r="A172" s="6"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D172" s="6"/>
       <c r="E172" s="6"/>
@@ -11608,7 +11605,7 @@
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
       <c r="D174" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E174" s="6"/>
       <c r="F174" s="6"/>
@@ -11616,7 +11613,7 @@
       <c r="H174" s="6"/>
       <c r="I174" s="6"/>
       <c r="J174" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K174" s="6"/>
       <c r="L174" s="6"/>
@@ -11656,7 +11653,7 @@
       <c r="H175" s="6"/>
       <c r="I175" s="6"/>
       <c r="J175" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K175" s="6"/>
       <c r="L175" s="6"/>
@@ -11688,7 +11685,7 @@
       <c r="B176" s="6"/>
       <c r="C176" s="6"/>
       <c r="D176" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E176" s="6"/>
       <c r="F176" s="6"/>
@@ -11727,7 +11724,7 @@
       <c r="C177" s="6"/>
       <c r="D177" s="6"/>
       <c r="E177" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F177" s="6"/>
       <c r="G177" s="6"/>
@@ -11736,7 +11733,7 @@
         <v>53</v>
       </c>
       <c r="J177" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K177" s="6"/>
       <c r="L177" s="6"/>
@@ -11769,13 +11766,13 @@
       <c r="C178" s="6"/>
       <c r="D178" s="6"/>
       <c r="E178" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F178" s="6"/>
       <c r="G178" s="6"/>
       <c r="H178" s="6"/>
       <c r="I178" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J178" s="6"/>
       <c r="K178" s="6"/>
@@ -11809,13 +11806,13 @@
       <c r="C179" s="6"/>
       <c r="D179" s="6"/>
       <c r="E179" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F179" s="6"/>
       <c r="G179" s="6"/>
       <c r="H179" s="6"/>
       <c r="I179" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J179" s="6"/>
       <c r="K179" s="6"/>
@@ -11849,13 +11846,13 @@
       <c r="C180" s="6"/>
       <c r="D180" s="6"/>
       <c r="E180" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F180" s="6"/>
       <c r="G180" s="6"/>
       <c r="H180" s="6"/>
       <c r="I180" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J180" s="6"/>
       <c r="K180" s="6"/>
@@ -11889,13 +11886,13 @@
       <c r="C181" s="6"/>
       <c r="D181" s="6"/>
       <c r="E181" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F181" s="6"/>
       <c r="G181" s="6"/>
       <c r="H181" s="6"/>
       <c r="I181" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J181" s="6"/>
       <c r="K181" s="6"/>
@@ -11935,10 +11932,10 @@
       <c r="G182" s="6"/>
       <c r="H182" s="6"/>
       <c r="I182" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J182" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K182" s="6"/>
       <c r="L182" s="6"/>
@@ -11970,7 +11967,7 @@
       <c r="B183" s="6"/>
       <c r="C183" s="6"/>
       <c r="D183" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E183" s="6"/>
       <c r="F183" s="6"/>
@@ -12047,7 +12044,7 @@
       <c r="C185" s="6"/>
       <c r="D185" s="6"/>
       <c r="E185" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F185" s="6"/>
       <c r="G185" s="6"/>
@@ -12085,7 +12082,7 @@
       <c r="C186" s="6"/>
       <c r="D186" s="6"/>
       <c r="E186" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F186" s="6"/>
       <c r="G186" s="6"/>
@@ -12122,7 +12119,7 @@
       <c r="B187" s="6"/>
       <c r="C187" s="6"/>
       <c r="D187" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E187" s="6"/>
       <c r="F187" s="6"/>
@@ -12199,7 +12196,7 @@
       <c r="C189" s="6"/>
       <c r="D189" s="6"/>
       <c r="E189" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F189" s="6"/>
       <c r="G189" s="6"/>
@@ -12237,13 +12234,13 @@
       <c r="C190" s="6"/>
       <c r="D190" s="6"/>
       <c r="E190" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F190" s="6"/>
       <c r="G190" s="6"/>
       <c r="H190" s="6"/>
       <c r="I190" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J190" s="6"/>
       <c r="K190" s="6"/>
@@ -12276,7 +12273,7 @@
       <c r="B191" s="6"/>
       <c r="C191" s="6"/>
       <c r="D191" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E191" s="6"/>
       <c r="F191" s="6"/>
@@ -12389,7 +12386,7 @@
       <c r="A194" s="6"/>
       <c r="B194" s="6"/>
       <c r="C194" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D194" s="6"/>
       <c r="E194" s="6"/>
@@ -12466,7 +12463,7 @@
       <c r="B196" s="6"/>
       <c r="C196" s="6"/>
       <c r="D196" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E196" s="6"/>
       <c r="F196" s="6"/>
@@ -12504,7 +12501,7 @@
       <c r="B197" s="6"/>
       <c r="C197" s="6"/>
       <c r="D197" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E197" s="6"/>
       <c r="F197" s="6"/>
@@ -12542,7 +12539,7 @@
       <c r="B198" s="6"/>
       <c r="C198" s="6"/>
       <c r="D198" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E198" s="6"/>
       <c r="F198" s="6"/>
@@ -12580,7 +12577,7 @@
       <c r="B199" s="6"/>
       <c r="C199" s="6"/>
       <c r="D199" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E199" s="6"/>
       <c r="F199" s="6"/>
@@ -12618,7 +12615,7 @@
       <c r="B200" s="6"/>
       <c r="C200" s="6"/>
       <c r="D200" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E200" s="6"/>
       <c r="F200" s="6"/>
@@ -12656,7 +12653,7 @@
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
       <c r="D201" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E201" s="6"/>
       <c r="F201" s="6"/>
@@ -12694,7 +12691,7 @@
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
       <c r="D202" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E202" s="6"/>
       <c r="F202" s="6"/>
@@ -12805,7 +12802,7 @@
       <c r="A205" s="6"/>
       <c r="B205" s="6"/>
       <c r="C205" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D205" s="6"/>
       <c r="E205" s="6"/>
@@ -12882,7 +12879,7 @@
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
       <c r="D207" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E207" s="6"/>
       <c r="F207" s="6"/>
@@ -12920,7 +12917,7 @@
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
       <c r="D208" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E208" s="6"/>
       <c r="F208" s="6"/>
@@ -12959,7 +12956,7 @@
       <c r="C209" s="6"/>
       <c r="D209" s="6"/>
       <c r="E209" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F209" s="6"/>
       <c r="G209" s="6"/>
@@ -12967,7 +12964,7 @@
       <c r="I209" s="6"/>
       <c r="J209" s="6"/>
       <c r="K209" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L209" s="6"/>
       <c r="M209" s="6"/>
@@ -12999,7 +12996,7 @@
       <c r="C210" s="6"/>
       <c r="D210" s="6"/>
       <c r="E210" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F210" s="6"/>
       <c r="G210" s="6"/>
@@ -13047,7 +13044,7 @@
       <c r="I211" s="6"/>
       <c r="J211" s="6"/>
       <c r="K211" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L211" s="6"/>
       <c r="M211" s="6"/>
@@ -13079,7 +13076,7 @@
       <c r="C212" s="6"/>
       <c r="D212" s="6"/>
       <c r="E212" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F212" s="6"/>
       <c r="G212" s="6"/>
@@ -13087,7 +13084,7 @@
       <c r="I212" s="6"/>
       <c r="J212" s="6"/>
       <c r="K212" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L212" s="6"/>
       <c r="M212" s="6"/>
@@ -13165,7 +13162,7 @@
       <c r="I214" s="6"/>
       <c r="J214" s="6"/>
       <c r="K214" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L214" s="6"/>
       <c r="M214" s="6"/>
@@ -13207,7 +13204,7 @@
       </c>
       <c r="J215" s="6"/>
       <c r="K215" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L215" s="6"/>
       <c r="M215" s="6"/>
@@ -13249,7 +13246,7 @@
       </c>
       <c r="J216" s="6"/>
       <c r="K216" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L216" s="6"/>
       <c r="M216" s="6"/>
@@ -13291,7 +13288,7 @@
       </c>
       <c r="J217" s="6"/>
       <c r="K217" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L217" s="6"/>
       <c r="M217" s="6"/>
@@ -13333,7 +13330,7 @@
       </c>
       <c r="J218" s="6"/>
       <c r="K218" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L218" s="6"/>
       <c r="M218" s="6"/>
@@ -13365,7 +13362,7 @@
       <c r="C219" s="6"/>
       <c r="D219" s="10"/>
       <c r="E219" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F219" s="6"/>
       <c r="G219" s="6"/>
@@ -13437,7 +13434,7 @@
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B221" s="6" t="s">
         <v>20</v>
@@ -13479,7 +13476,7 @@
       <c r="A222" s="6"/>
       <c r="B222" s="6"/>
       <c r="C222" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D222" s="6"/>
       <c r="E222" s="6"/>
@@ -13555,7 +13552,7 @@
       <c r="A224" s="6"/>
       <c r="B224" s="6"/>
       <c r="C224" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D224" s="6"/>
       <c r="E224" s="6"/>
@@ -13593,7 +13590,7 @@
       <c r="A225" s="6"/>
       <c r="B225" s="6"/>
       <c r="C225" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D225" s="6"/>
       <c r="E225" s="6"/>
@@ -13640,7 +13637,7 @@
       <c r="H226" s="6"/>
       <c r="I226" s="6"/>
       <c r="J226" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K226" s="6"/>
       <c r="L226" s="6"/>
@@ -13671,7 +13668,7 @@
       <c r="A227" s="6"/>
       <c r="B227" s="6"/>
       <c r="C227" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D227" s="6"/>
       <c r="E227" s="6"/>
@@ -13748,7 +13745,7 @@
       <c r="B229" s="6"/>
       <c r="C229" s="6"/>
       <c r="D229" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E229" s="6"/>
       <c r="F229" s="6"/>
@@ -13794,7 +13791,7 @@
       <c r="H230" s="6"/>
       <c r="I230" s="6"/>
       <c r="J230" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K230" s="6"/>
       <c r="L230" s="6"/>
@@ -13864,7 +13861,7 @@
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
       <c r="D232" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E232" s="6"/>
       <c r="F232" s="6"/>
@@ -13941,7 +13938,7 @@
       <c r="C234" s="6"/>
       <c r="D234" s="6"/>
       <c r="E234" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F234" s="6"/>
       <c r="G234" s="6"/>
@@ -13979,7 +13976,7 @@
       <c r="C235" s="6"/>
       <c r="D235" s="6"/>
       <c r="E235" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F235" s="6"/>
       <c r="G235" s="6"/>
@@ -14016,7 +14013,7 @@
       <c r="B236" s="6"/>
       <c r="C236" s="6"/>
       <c r="D236" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E236" s="6"/>
       <c r="F236" s="6"/>
@@ -14093,13 +14090,13 @@
       <c r="C238" s="6"/>
       <c r="D238" s="6"/>
       <c r="E238" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F238" s="6"/>
       <c r="G238" s="6"/>
       <c r="H238" s="6"/>
       <c r="I238" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J238" s="6"/>
       <c r="K238" s="6"/>
@@ -14133,13 +14130,13 @@
       <c r="C239" s="6"/>
       <c r="D239" s="6"/>
       <c r="E239" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F239" s="6"/>
       <c r="G239" s="6"/>
       <c r="H239" s="6"/>
       <c r="I239" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J239" s="6"/>
       <c r="K239" s="6"/>
@@ -14172,7 +14169,7 @@
       <c r="B240" s="6"/>
       <c r="C240" s="6"/>
       <c r="D240" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E240" s="6"/>
       <c r="F240" s="6"/>
@@ -14285,7 +14282,7 @@
       <c r="A243" s="6"/>
       <c r="B243" s="6"/>
       <c r="C243" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D243" s="6"/>
       <c r="E243" s="6"/>
@@ -14362,7 +14359,7 @@
       <c r="B245" s="6"/>
       <c r="C245" s="6"/>
       <c r="D245" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E245" s="6"/>
       <c r="F245" s="6"/>
@@ -14473,7 +14470,7 @@
       <c r="A248" s="6"/>
       <c r="B248" s="6"/>
       <c r="C248" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D248" s="6"/>
       <c r="E248" s="6"/>
@@ -14550,7 +14547,7 @@
       <c r="B250" s="6"/>
       <c r="C250" s="6"/>
       <c r="D250" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E250" s="6"/>
       <c r="F250" s="6"/>
@@ -14588,7 +14585,7 @@
       <c r="B251" s="6"/>
       <c r="C251" s="6"/>
       <c r="D251" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E251" s="6"/>
       <c r="F251" s="6"/>
@@ -14627,7 +14624,7 @@
       <c r="C252" s="6"/>
       <c r="D252" s="6"/>
       <c r="E252" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F252" s="6"/>
       <c r="G252" s="6"/>
@@ -14635,7 +14632,7 @@
       <c r="I252" s="6"/>
       <c r="J252" s="6"/>
       <c r="K252" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
@@ -14667,7 +14664,7 @@
       <c r="C253" s="6"/>
       <c r="D253" s="6"/>
       <c r="E253" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F253" s="6"/>
       <c r="G253" s="6"/>
@@ -14715,7 +14712,7 @@
       <c r="I254" s="6"/>
       <c r="J254" s="6"/>
       <c r="K254" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
@@ -14747,7 +14744,7 @@
       <c r="C255" s="6"/>
       <c r="D255" s="6"/>
       <c r="E255" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F255" s="6"/>
       <c r="G255" s="6"/>
@@ -14755,7 +14752,7 @@
       <c r="I255" s="6"/>
       <c r="J255" s="6"/>
       <c r="K255" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
@@ -14833,7 +14830,7 @@
       <c r="I257" s="6"/>
       <c r="J257" s="6"/>
       <c r="K257" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
@@ -14875,7 +14872,7 @@
       </c>
       <c r="J258" s="6"/>
       <c r="K258" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
@@ -14917,7 +14914,7 @@
       </c>
       <c r="J259" s="6"/>
       <c r="K259" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
@@ -14959,7 +14956,7 @@
       </c>
       <c r="J260" s="6"/>
       <c r="K260" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
@@ -15001,7 +14998,7 @@
       </c>
       <c r="J261" s="6"/>
       <c r="K261" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
@@ -15033,7 +15030,7 @@
       <c r="C262" s="6"/>
       <c r="D262" s="6"/>
       <c r="E262" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F262" s="6"/>
       <c r="G262" s="6"/>
@@ -15069,7 +15066,7 @@
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B263" s="6" t="s">
         <v>20</v>
@@ -15111,7 +15108,7 @@
       <c r="A264" s="6"/>
       <c r="B264" s="6"/>
       <c r="C264" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D264" s="6"/>
       <c r="E264" s="6"/>
@@ -15187,7 +15184,7 @@
       <c r="A266" s="6"/>
       <c r="B266" s="6"/>
       <c r="C266" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D266" s="6"/>
       <c r="E266" s="6"/>
@@ -15236,7 +15233,7 @@
         <v>57</v>
       </c>
       <c r="J267" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K267" s="6"/>
       <c r="L267" s="6"/>
@@ -15267,7 +15264,7 @@
       <c r="A268" s="6"/>
       <c r="B268" s="6"/>
       <c r="C268" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D268" s="6"/>
       <c r="E268" s="6"/>
@@ -15344,7 +15341,7 @@
       <c r="B270" s="6"/>
       <c r="C270" s="6"/>
       <c r="D270" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E270" s="6"/>
       <c r="F270" s="6"/>
@@ -15390,7 +15387,7 @@
       <c r="H271" s="6"/>
       <c r="I271" s="6"/>
       <c r="J271" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K271" s="6"/>
       <c r="L271" s="6"/>
@@ -15460,7 +15457,7 @@
       <c r="B273" s="6"/>
       <c r="C273" s="6"/>
       <c r="D273" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E273" s="6"/>
       <c r="F273" s="6"/>
@@ -15468,7 +15465,7 @@
       <c r="H273" s="6"/>
       <c r="I273" s="6"/>
       <c r="J273" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K273" s="6"/>
       <c r="L273" s="6"/>
@@ -15501,7 +15498,7 @@
       <c r="C274" s="6"/>
       <c r="D274" s="6"/>
       <c r="E274" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F274" s="6"/>
       <c r="G274" s="6"/>
@@ -15541,7 +15538,7 @@
       <c r="C275" s="6"/>
       <c r="D275" s="6"/>
       <c r="E275" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F275" s="6"/>
       <c r="G275" s="6"/>
@@ -15581,7 +15578,7 @@
       <c r="C276" s="6"/>
       <c r="D276" s="6"/>
       <c r="E276" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F276" s="6"/>
       <c r="G276" s="6"/>
@@ -15621,7 +15618,7 @@
       <c r="C277" s="6"/>
       <c r="D277" s="6"/>
       <c r="E277" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F277" s="6"/>
       <c r="G277" s="6"/>
@@ -15696,7 +15693,7 @@
       <c r="B279" s="6"/>
       <c r="C279" s="6"/>
       <c r="D279" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E279" s="6"/>
       <c r="F279" s="6"/>
@@ -15735,7 +15732,7 @@
       <c r="C280" s="6"/>
       <c r="D280" s="6"/>
       <c r="E280" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F280" s="6"/>
       <c r="G280" s="6"/>
@@ -15775,13 +15772,13 @@
       <c r="C281" s="6"/>
       <c r="D281" s="6"/>
       <c r="E281" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F281" s="6"/>
       <c r="G281" s="6"/>
       <c r="H281" s="6"/>
       <c r="I281" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J281" s="6"/>
       <c r="K281" s="6"/>
@@ -15815,7 +15812,7 @@
       <c r="C282" s="6"/>
       <c r="D282" s="6"/>
       <c r="E282" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F282" s="6"/>
       <c r="G282" s="6"/>
@@ -15855,7 +15852,7 @@
       <c r="C283" s="6"/>
       <c r="D283" s="6"/>
       <c r="E283" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F283" s="6"/>
       <c r="G283" s="6"/>
@@ -15894,7 +15891,7 @@
       <c r="B284" s="6"/>
       <c r="C284" s="6"/>
       <c r="D284" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E284" s="6"/>
       <c r="F284" s="6"/>
@@ -15933,7 +15930,7 @@
       <c r="C285" s="6"/>
       <c r="D285" s="6"/>
       <c r="E285" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F285" s="6"/>
       <c r="G285" s="6"/>
@@ -15972,7 +15969,7 @@
       <c r="B286" s="6"/>
       <c r="C286" s="6"/>
       <c r="D286" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E286" s="6"/>
       <c r="F286" s="6"/>
@@ -16049,7 +16046,7 @@
       <c r="C288" s="6"/>
       <c r="D288" s="6"/>
       <c r="E288" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F288" s="6"/>
       <c r="G288" s="6"/>
@@ -16087,7 +16084,7 @@
       <c r="C289" s="6"/>
       <c r="D289" s="6"/>
       <c r="E289" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F289" s="6"/>
       <c r="G289" s="6"/>
@@ -16124,7 +16121,7 @@
       <c r="B290" s="6"/>
       <c r="C290" s="6"/>
       <c r="D290" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E290" s="6"/>
       <c r="F290" s="6"/>
@@ -16201,7 +16198,7 @@
       <c r="C292" s="6"/>
       <c r="D292" s="6"/>
       <c r="E292" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F292" s="6"/>
       <c r="G292" s="6"/>
@@ -16239,13 +16236,13 @@
       <c r="C293" s="6"/>
       <c r="D293" s="6"/>
       <c r="E293" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F293" s="6"/>
       <c r="G293" s="6"/>
       <c r="H293" s="6"/>
       <c r="I293" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J293" s="6"/>
       <c r="K293" s="6"/>
@@ -16278,7 +16275,7 @@
       <c r="B294" s="6"/>
       <c r="C294" s="6"/>
       <c r="D294" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E294" s="6"/>
       <c r="F294" s="6"/>
@@ -16391,7 +16388,7 @@
       <c r="A297" s="6"/>
       <c r="B297" s="6"/>
       <c r="C297" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D297" s="6"/>
       <c r="E297" s="6"/>
@@ -16468,7 +16465,7 @@
       <c r="B299" s="6"/>
       <c r="C299" s="6"/>
       <c r="D299" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E299" s="6"/>
       <c r="F299" s="6"/>
@@ -46666,7 +46663,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>88</v>
@@ -46677,7 +46674,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46688,12 +46685,12 @@
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
@@ -46701,15 +46698,15 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46720,21 +46717,21 @@
         <v>5</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46745,12 +46742,12 @@
         <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>8</v>
@@ -46783,7 +46780,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>88</v>
@@ -46819,7 +46816,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46832,7 +46829,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>5</v>
@@ -46849,7 +46846,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>20</v>
@@ -46858,19 +46855,19 @@
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
       <c r="D7" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8"/>
       <c r="D8" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46890,42 +46887,42 @@
         <v>72</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8"/>
       <c r="D12" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="4" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46936,30 +46933,30 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
       <c r="E19" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
       <c r="E20" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46972,7 +46969,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>5</v>
@@ -46998,7 +46995,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>8</v>
@@ -47008,7 +47005,7 @@
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>13</v>
@@ -47017,7 +47014,7 @@
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>8</v>
@@ -47025,7 +47022,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>20</v>
@@ -47034,30 +47031,30 @@
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
       <c r="D30" s="4" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="E30" s="4"/>
       <c r="G30" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
       <c r="D31" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E31" s="4"/>
       <c r="G31" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -47096,7 +47093,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>88</v>
@@ -47111,7 +47108,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -47132,7 +47129,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47143,7 +47140,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47154,12 +47151,12 @@
         <v>10</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47188,7 +47185,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>20</v>
@@ -47205,12 +47202,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>283</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47239,7 +47236,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>8</v>
@@ -47247,7 +47244,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>8</v>
@@ -47261,12 +47258,12 @@
         <v>13</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>20</v>
@@ -47282,12 +47279,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>288</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47316,7 +47313,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>20</v>
@@ -47334,7 +47331,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47363,7 +47360,7 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>20</v>
@@ -47381,7 +47378,7 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C41" s="4"/>
     </row>
@@ -47425,12 +47422,12 @@
         <v>13</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>20</v>
@@ -47454,7 +47451,7 @@
         <v>107</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47463,7 +47460,7 @@
         <v>108</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47472,7 +47469,7 @@
         <v>109</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47482,18 +47479,18 @@
         <v>110</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F55" s="4"/>
     </row>
@@ -47507,14 +47504,14 @@
       <c r="A57" s="4"/>
       <c r="E57" s="6"/>
       <c r="F57" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
       <c r="E58" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -47531,7 +47528,7 @@
       <c r="A60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G60" s="4"/>
     </row>
@@ -47539,7 +47536,7 @@
       <c r="B61" s="7"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47567,7 +47564,7 @@
         <v>107</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47576,7 +47573,7 @@
         <v>108</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47585,7 +47582,7 @@
         <v>109</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47594,21 +47591,21 @@
         <v>110</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F69" s="7"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="H70" s="4" t="s">
         <v>295</v>
-      </c>
-      <c r="H70" s="4" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -47643,13 +47640,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -47677,7 +47674,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47696,7 +47693,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47709,7 +47706,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
@@ -47723,12 +47720,12 @@
         <v>13</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47749,7 +47746,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>8</v>
@@ -47764,12 +47761,12 @@
         <v>10</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>10</v>
@@ -47777,7 +47774,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>10</v>
@@ -47785,18 +47782,18 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>8</v>
@@ -47810,7 +47807,7 @@
         <v>13</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47825,7 +47822,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47854,7 +47851,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>8</v>
@@ -47862,15 +47859,15 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>310</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>13</v>
@@ -47878,10 +47875,10 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>312</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -47914,13 +47911,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -47950,7 +47947,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47963,7 +47960,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>5</v>
@@ -48003,7 +48000,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>13</v>

</xml_diff>